<commit_message>
Broke out the options to multiple files
</commit_message>
<xml_diff>
--- a/Meraki/ACLs/L_634444597505861201.xlsx
+++ b/Meraki/ACLs/L_634444597505861201.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsimmon8/Automation Projects/Toddomation/Toddomation/Meraki/ACLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B4BEF0-08F2-2F46-8040-F05283202D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A76E22-4733-ED46-A23D-CB79E8DE63B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="500" windowWidth="17960" windowHeight="12340" activeTab="2" xr2:uid="{C7553D00-AF08-44BD-93AF-2C2EDD8637EA}"/>
+    <workbookView xWindow="120" yWindow="500" windowWidth="17960" windowHeight="12340" xr2:uid="{C7553D00-AF08-44BD-93AF-2C2EDD8637EA}"/>
   </bookViews>
   <sheets>
-    <sheet name="SwitchACL" sheetId="1" r:id="rId1"/>
-    <sheet name="FirewallL3OutACL" sheetId="3" r:id="rId2"/>
-    <sheet name="FirewallL3InACL" sheetId="6" r:id="rId3"/>
+    <sheet name="FirewallL3OutACL" sheetId="3" r:id="rId1"/>
+    <sheet name="FirewallL3InACL" sheetId="6" r:id="rId2"/>
+    <sheet name="SwitchACL" sheetId="1" r:id="rId3"/>
     <sheet name="WirelessACL" sheetId="5" r:id="rId4"/>
     <sheet name="Validation" sheetId="2" r:id="rId5"/>
   </sheets>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="62">
   <si>
     <t>policy</t>
   </si>
@@ -183,12 +183,6 @@
     <t>3</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Deny SSH from subnet</t>
   </si>
   <si>
@@ -229,6 +223,9 @@
   </si>
   <si>
     <t>Allow HTTPS</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -586,292 +583,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341B248C-3085-4936-8578-6445EAEAAD13}">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5" customWidth="1"/>
-    <col min="8" max="8" width="9.83203125" customWidth="1"/>
-    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2">
-        <v>22</v>
-      </c>
-      <c r="H2">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3">
-        <v>21</v>
-      </c>
-      <c r="H3">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>443</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>53</v>
-      </c>
-      <c r="H8" t="s">
-        <v>12</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B7088EA-612F-454E-9891-4248A9BFC3CD}">
-          <x14:formula1>
-            <xm:f>Validation!$A$2:$A$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>A2:A8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02C76058-A249-4BA9-ABE5-330BCE6C96D3}">
-          <x14:formula1>
-            <xm:f>Validation!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B8</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5259161A-E096-45BF-ACBF-CF51B510A2F8}">
-          <x14:formula1>
-            <xm:f>Validation!$C$2:$C$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C8</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B094927E-4958-4C24-B573-F1E357B002D2}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -922,7 +637,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
@@ -948,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
@@ -980,7 +695,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1">
         <v>22</v>
@@ -1006,7 +721,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1">
         <v>21</v>
@@ -1048,11 +763,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9E1B22-FEFE-964E-A087-DE2BD48B00C8}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -1109,7 +824,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F2" s="1">
         <v>22</v>
@@ -1135,7 +850,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F3" s="1">
         <v>21</v>
@@ -1155,7 +870,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -1181,7 +896,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -1207,22 +922,22 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1233,22 +948,22 @@
         <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>25</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1284,12 +999,294 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{341B248C-3085-4936-8578-6445EAEAAD13}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="9.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>443</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2B7088EA-612F-454E-9891-4248A9BFC3CD}">
+          <x14:formula1>
+            <xm:f>Validation!$A$2:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2:A8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{02C76058-A249-4BA9-ABE5-330BCE6C96D3}">
+          <x14:formula1>
+            <xm:f>Validation!$B$2:$B$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5259161A-E096-45BF-ACBF-CF51B510A2F8}">
+          <x14:formula1>
+            <xm:f>Validation!$C$2:$C$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>C2:C8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244C9E28-B55E-455C-AE61-F26CCA69015F}">
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J11" sqref="J11:J13"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1514,7 +1511,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1546,7 +1543,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
@@ -1578,7 +1575,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>15</v>
@@ -1610,7 +1607,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>15</v>
@@ -1636,16 +1633,13 @@
       <c r="I10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="K10" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
@@ -1677,7 +1671,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -1709,7 +1703,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>15</v>
@@ -1750,25 +1744,25 @@
           <x14:formula1>
             <xm:f>Validation!$D$2:$D$3</xm:f>
           </x14:formula1>
-          <xm:sqref>F14:F99</xm:sqref>
+          <xm:sqref>F14:F86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C4DC42B-675C-43BD-8514-496C1798B265}">
           <x14:formula1>
             <xm:f>Validation!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B99</xm:sqref>
+          <xm:sqref>B2:B86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{89DBB352-C36A-437C-AE9B-B91A1863DD51}">
           <x14:formula1>
             <xm:f>Validation!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C99</xm:sqref>
+          <xm:sqref>C2:C86</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7B7B4E20-6A08-42F7-BCC5-1D1AA0C31A56}">
           <x14:formula1>
             <xm:f>Validation!$E$2:$E$6</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D99</xm:sqref>
+          <xm:sqref>D2:D86</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>